<commit_message>
Hatların sağ ve solda olma durumunun tespiti sağlandı
</commit_message>
<xml_diff>
--- a/output/CORLU 380 HADIMKOY GIS(1).xlsx
+++ b/output/CORLU 380 HADIMKOY GIS(1).xlsx
@@ -780,7 +780,7 @@
         <v>7</v>
       </c>
       <c r="D17">
-        <v>176.8</v>
+        <v>-176.8</v>
       </c>
       <c r="E17" t="s">
         <v>7</v>
@@ -803,7 +803,7 @@
         <v>7</v>
       </c>
       <c r="D18">
-        <v>709.87</v>
+        <v>-709.87</v>
       </c>
       <c r="E18" t="s">
         <v>7</v>

</xml_diff>

<commit_message>
Hata giderme Yöne bağlı olarak hatalı hesaplama yapma sorunu giderildi.
</commit_message>
<xml_diff>
--- a/output/CORLU 380 HADIMKOY GIS(1).xlsx
+++ b/output/CORLU 380 HADIMKOY GIS(1).xlsx
@@ -435,13 +435,13 @@
         <v>7</v>
       </c>
       <c r="D2">
-        <v>828.64</v>
+        <v>105.85</v>
       </c>
       <c r="E2" t="s">
         <v>7</v>
       </c>
       <c r="F2">
-        <v>440.8</v>
+        <v>56.35</v>
       </c>
       <c r="G2" t="s">
         <v>7</v>
@@ -458,13 +458,13 @@
         <v>7</v>
       </c>
       <c r="D3">
-        <v>828.05</v>
+        <v>105.61</v>
       </c>
       <c r="E3" t="s">
         <v>7</v>
       </c>
       <c r="F3">
-        <v>439.7</v>
+        <v>56.12</v>
       </c>
       <c r="G3" t="s">
         <v>7</v>
@@ -481,13 +481,13 @@
         <v>7</v>
       </c>
       <c r="D4">
-        <v>827.39</v>
+        <v>105.37</v>
       </c>
       <c r="E4" t="s">
         <v>7</v>
       </c>
       <c r="F4">
-        <v>438.59</v>
+        <v>55.9</v>
       </c>
       <c r="G4" t="s">
         <v>7</v>
@@ -504,13 +504,13 @@
         <v>7</v>
       </c>
       <c r="D5">
-        <v>826.74</v>
+        <v>105.13</v>
       </c>
       <c r="E5" t="s">
         <v>7</v>
       </c>
       <c r="F5">
-        <v>437.47</v>
+        <v>55.67</v>
       </c>
       <c r="G5" t="s">
         <v>7</v>
@@ -527,13 +527,13 @@
         <v>7</v>
       </c>
       <c r="D6">
-        <v>826.08</v>
+        <v>104.89</v>
       </c>
       <c r="E6" t="s">
         <v>7</v>
       </c>
       <c r="F6">
-        <v>436.36</v>
+        <v>55.45</v>
       </c>
       <c r="G6" t="s">
         <v>7</v>
@@ -550,13 +550,13 @@
         <v>7</v>
       </c>
       <c r="D7">
-        <v>344.22</v>
+        <v>183.3</v>
       </c>
       <c r="E7" t="s">
         <v>7</v>
       </c>
       <c r="F7">
-        <v>249.83</v>
+        <v>133.13</v>
       </c>
       <c r="G7" t="s">
         <v>7</v>
@@ -596,13 +596,13 @@
         <v>7</v>
       </c>
       <c r="D9">
-        <v>660.64</v>
+        <v>985.61</v>
       </c>
       <c r="E9" t="s">
         <v>7</v>
       </c>
       <c r="F9">
-        <v>593.03</v>
+        <v>885.63</v>
       </c>
       <c r="G9" t="s">
         <v>7</v>
@@ -619,13 +619,13 @@
         <v>7</v>
       </c>
       <c r="D10">
-        <v>298.64</v>
+        <v>285.65</v>
       </c>
       <c r="E10" t="s">
         <v>7</v>
       </c>
       <c r="F10">
-        <v>244.51</v>
+        <v>233.98</v>
       </c>
       <c r="G10" t="s">
         <v>7</v>
@@ -642,13 +642,13 @@
         <v>7</v>
       </c>
       <c r="D11">
-        <v>148.61</v>
+        <v>142.27</v>
       </c>
       <c r="E11" t="s">
         <v>7</v>
       </c>
       <c r="F11">
-        <v>95.26000000000001</v>
+        <v>91.17</v>
       </c>
       <c r="G11" t="s">
         <v>7</v>
@@ -665,13 +665,13 @@
         <v>7</v>
       </c>
       <c r="D12">
-        <v>111.98</v>
+        <v>110.43</v>
       </c>
       <c r="E12" t="s">
         <v>7</v>
       </c>
       <c r="F12">
-        <v>61.11</v>
+        <v>60.26</v>
       </c>
       <c r="G12" t="s">
         <v>7</v>
@@ -688,13 +688,13 @@
         <v>7</v>
       </c>
       <c r="D13">
-        <v>112.72</v>
+        <v>111.17</v>
       </c>
       <c r="E13" t="s">
         <v>7</v>
       </c>
       <c r="F13">
-        <v>61.04</v>
+        <v>60.19</v>
       </c>
       <c r="G13" t="s">
         <v>7</v>
@@ -711,13 +711,13 @@
         <v>7</v>
       </c>
       <c r="D14">
-        <v>111.68</v>
+        <v>110.15</v>
       </c>
       <c r="E14" t="s">
         <v>7</v>
       </c>
       <c r="F14">
-        <v>60.97</v>
+        <v>60.13</v>
       </c>
       <c r="G14" t="s">
         <v>7</v>
@@ -734,13 +734,13 @@
         <v>7</v>
       </c>
       <c r="D15">
-        <v>112.06</v>
+        <v>110.49</v>
       </c>
       <c r="E15" t="s">
         <v>7</v>
       </c>
       <c r="F15">
-        <v>60.9</v>
+        <v>60.06</v>
       </c>
       <c r="G15" t="s">
         <v>7</v>
@@ -757,13 +757,13 @@
         <v>7</v>
       </c>
       <c r="D16">
-        <v>112.53</v>
+        <v>110.96</v>
       </c>
       <c r="E16" t="s">
         <v>7</v>
       </c>
       <c r="F16">
-        <v>60.84</v>
+        <v>59.99</v>
       </c>
       <c r="G16" t="s">
         <v>7</v>
@@ -780,13 +780,13 @@
         <v>7</v>
       </c>
       <c r="D17">
-        <v>-176.8</v>
+        <v>-191.33</v>
       </c>
       <c r="E17" t="s">
         <v>7</v>
       </c>
       <c r="F17">
-        <v>60.77</v>
+        <v>59.93</v>
       </c>
       <c r="G17" t="s">
         <v>7</v>
@@ -803,13 +803,13 @@
         <v>7</v>
       </c>
       <c r="D18">
-        <v>-709.87</v>
+        <v>-768.21</v>
       </c>
       <c r="E18" t="s">
         <v>7</v>
       </c>
       <c r="F18">
-        <v>60.7</v>
+        <v>59.86</v>
       </c>
       <c r="G18" t="s">
         <v>7</v>
@@ -832,7 +832,7 @@
         <v>7</v>
       </c>
       <c r="F19">
-        <v>99.03</v>
+        <v>90.90000000000001</v>
       </c>
       <c r="G19" t="s">
         <v>7</v>
@@ -855,7 +855,7 @@
         <v>7</v>
       </c>
       <c r="F20">
-        <v>546.37</v>
+        <v>501.5</v>
       </c>
       <c r="G20" t="s">
         <v>7</v>
@@ -878,7 +878,7 @@
         <v>7</v>
       </c>
       <c r="F21">
-        <v>993.64</v>
+        <v>912.05</v>
       </c>
       <c r="G21" t="s">
         <v>7</v>
@@ -901,7 +901,7 @@
         <v>7</v>
       </c>
       <c r="F22">
-        <v>924.39</v>
+        <v>939.21</v>
       </c>
       <c r="G22" t="s">
         <v>7</v>
@@ -924,7 +924,7 @@
         <v>7</v>
       </c>
       <c r="F23">
-        <v>748.1799999999999</v>
+        <v>760.1900000000001</v>
       </c>
       <c r="G23" t="s">
         <v>7</v>
@@ -947,7 +947,7 @@
         <v>7</v>
       </c>
       <c r="F24">
-        <v>571.96</v>
+        <v>581.16</v>
       </c>
       <c r="G24" t="s">
         <v>7</v>
@@ -970,7 +970,7 @@
         <v>7</v>
       </c>
       <c r="F25">
-        <v>395.75</v>
+        <v>402.12</v>
       </c>
       <c r="G25" t="s">
         <v>7</v>
@@ -993,7 +993,7 @@
         <v>7</v>
       </c>
       <c r="F26">
-        <v>219.53</v>
+        <v>223.07</v>
       </c>
       <c r="G26" t="s">
         <v>7</v>

</xml_diff>